<commit_message>
another commit from mark
</commit_message>
<xml_diff>
--- a/Jira Scripting Plan_v2_3.xlsx
+++ b/Jira Scripting Plan_v2_3.xlsx
@@ -2428,7 +2428,7 @@
       <pane xSplit="6" ySplit="2" topLeftCell="H25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="M29" sqref="M29"/>
+      <selection pane="bottomRight" activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="23" customHeight="1" x14ac:dyDescent="0"/>
@@ -4188,7 +4188,7 @@
         <v>2</v>
       </c>
       <c r="L28" s="3" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="M28" s="20" t="s">
         <v>28</v>

</xml_diff>